<commit_message>
lab1: divide some logic from `Program.cs` into separate files
</commit_message>
<xml_diff>
--- a/lab1/report/графики.xlsx
+++ b/lab1/report/графики.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Univer\AI\lab1\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syche\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F877759-5188-4AFA-B221-2D6B603ED2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32000DD5-B086-4C4B-AF84-CE2DFAA8E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13065" yWindow="4935" windowWidth="20565" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
   <si>
     <t>b*</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Max C: 2958</t>
+  </si>
+  <si>
+    <t>A* с эвристикой 1</t>
+  </si>
+  <si>
+    <t>A* с эвристикой 3</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +333,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -590,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,6 +682,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,9 +698,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,7 +754,6 @@
               <a:rPr lang="ru-RU"/>
               <a:t>Итерации</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -773,13 +790,80 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Поиск в ширину</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>33.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1628.2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>23217</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1830-47E3-9848-D4829FD283B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Двунаправленный</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -791,19 +875,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -831,18 +903,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$E$3</c:f>
+              <c:f>Sheet1!$C$6:$G$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1354.8</c:v>
+                  <c:v>13.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46360</c:v>
+                  <c:v>79.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>626.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4654.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,92 +928,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1144-48A6-8ACC-861D96C0E276}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Двунаправленный</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$G$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$6:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>541.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4891.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1144-48A6-8ACC-861D96C0E276}"/>
+              <c16:uniqueId val="{00000004-1830-47E3-9848-D4829FD283B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -943,7 +936,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Эвристика 1</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* с эвристикой 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -955,19 +956,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1014,7 +1003,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1144-48A6-8ACC-861D96C0E276}"/>
+              <c16:uniqueId val="{00000005-1830-47E3-9848-D4829FD283B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1022,7 +1011,15 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Эвристика 3</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* с эвристикой 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1034,19 +1031,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1076,22 +1061,22 @@
             <c:numRef>
               <c:f>Sheet1!$C$12:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.7</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>308.7</c:v>
+                  <c:v>163.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3543</c:v>
+                  <c:v>1275.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,7 +1084,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-1144-48A6-8ACC-861D96C0E276}"/>
+              <c16:uniqueId val="{00000006-1830-47E3-9848-D4829FD283B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1111,13 +1096,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="353223136"/>
-        <c:axId val="353223968"/>
+        <c:axId val="354632832"/>
+        <c:axId val="354632416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="353223136"/>
+        <c:axId val="354632832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1160,7 +1144,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353223968"/>
+        <c:crossAx val="354632416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1168,9 +1152,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="353223968"/>
+        <c:axId val="354632416"/>
         <c:scaling>
-          <c:logBase val="11"/>
+          <c:logBase val="15"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1189,7 +1173,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1220,7 +1204,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353223136"/>
+        <c:crossAx val="354632832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1264,7 +1248,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1322,6 +1306,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Кол-во</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> узлов</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1355,7 +1369,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1373,19 +1387,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1413,18 +1415,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$E$4</c:f>
+              <c:f>Sheet1!$C$3:$E$3</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>212.5</c:v>
+                  <c:v>33.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7989.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>261348</c:v>
+                  <c:v>1628.2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>23217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1432,7 +1434,236 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C8E5-47F6-9F33-C4FF6FFDBC16}"/>
+              <c16:uniqueId val="{00000000-DEA7-418E-B210-C89F7419E9FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Двунаправленный</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>636.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5198.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37174.800000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEA7-418E-B210-C89F7419E9FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* с эвристикой 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1849.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41375.300000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DEA7-418E-B210-C89F7419E9FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* с эвристикой 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>223.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1120.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8842.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DEA7-418E-B210-C89F7419E9FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1444,13 +1675,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="581355568"/>
-        <c:axId val="581365552"/>
+        <c:axId val="708490336"/>
+        <c:axId val="708490752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="581355568"/>
+        <c:axId val="708490336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,7 +1723,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581365552"/>
+        <c:crossAx val="708490752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1501,8 +1731,591 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="581365552"/>
+        <c:axId val="708490752"/>
         <c:scaling>
+          <c:logBase val="11"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="708490336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>b*</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4011596675415573"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Поиск в ширину</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>13.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F9E4-4247-ACD8-F0C988E80C49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Двунаправленный</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F9E4-4247-ACD8-F0C988E80C49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* с эвристикой 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>14.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1762899999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.601560000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F9E4-4247-ACD8-F0C988E80C49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* с эвристикой 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>2.2400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F9E4-4247-ACD8-F0C988E80C49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="256252800"/>
+        <c:axId val="266578560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="256252800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266578560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="266578560"/>
+        <c:scaling>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1552,7 +2365,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581355568"/>
+        <c:crossAx val="256252800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1564,8 +2377,39 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1688,8 +2532,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1797,6 +2681,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1807,6 +2696,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1838,6 +2732,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2192,7 +3089,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2300,6 +3197,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2310,6 +3212,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2341,6 +3248,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2694,27 +3604,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>314068</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>118459</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>884981</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>75235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>149566</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>42761</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>224260</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>117675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C64372-EED6-436A-A662-5D049741A1CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F31F6B6B-FBD7-45B3-9FDB-5BE65BACE8EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2734,23 +4160,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>326939</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>192301</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>335592</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>137238</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>278027</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>39386</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>849504</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>24744</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EFDDAB1-5F71-4756-82AB-88EA8534744A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58DA6CEF-32F4-4756-B036-D29810B00F29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2763,6 +4189,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285009</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132309</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>339586</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>13903</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178A1BFD-11CF-4A3C-9D34-751555A7705E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3036,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V420"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="I12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,38 +4522,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="29"/>
+      <c r="B1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2">
         <v>2</v>
       </c>
@@ -3145,20 +4607,20 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="21">
-        <v>34.5</v>
-      </c>
-      <c r="D3" s="21">
-        <v>1354.8</v>
+      <c r="C3" s="26">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="D3" s="26">
+        <v>1628.2</v>
       </c>
       <c r="E3" s="22">
-        <v>46360</v>
+        <v>23217</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -3166,7 +4628,7 @@
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="30">
         <v>2</v>
       </c>
       <c r="L3" s="10" t="s">
@@ -3204,18 +4666,18 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="21">
-        <v>212.5</v>
-      </c>
-      <c r="D4" s="21">
-        <v>7989.1</v>
+      <c r="C4" s="26">
+        <v>205.7</v>
+      </c>
+      <c r="D4" s="26">
+        <v>9562.9</v>
       </c>
       <c r="E4" s="22">
-        <v>261348</v>
+        <v>134451</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -3223,7 +4685,7 @@
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="28"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="11" t="s">
         <v>7</v>
       </c>
@@ -3259,18 +4721,18 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="21">
-        <v>14.09</v>
+        <v>13.85</v>
       </c>
       <c r="D5" s="21">
-        <v>9.18</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="E5" s="22">
-        <v>3.89</v>
+        <v>6.88</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -3278,14 +4740,14 @@
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="31">
         <v>4</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="17">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="N5" s="18">
         <v>11</v>
@@ -3316,38 +4778,33 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="23">
-        <f>AVERAGE(M3:V3)</f>
+      <c r="C6" s="26">
         <v>2</v>
       </c>
-      <c r="D6" s="23">
-        <f>AVERAGE(M5:V5)</f>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="E6" s="23">
-        <f>AVERAGE(M7:V7)</f>
-        <v>72.7</v>
-      </c>
-      <c r="F6" s="1">
-        <f>AVERAGE(M9:V9)</f>
-        <v>541.6</v>
-      </c>
-      <c r="G6" s="1">
-        <f>AVERAGE(M11:V11)</f>
-        <v>4891.8</v>
-      </c>
-      <c r="K6" s="28"/>
+      <c r="D6" s="26">
+        <v>13.4</v>
+      </c>
+      <c r="E6" s="26">
+        <v>79.8</v>
+      </c>
+      <c r="F6" s="26">
+        <v>626.29999999999995</v>
+      </c>
+      <c r="G6" s="26">
+        <v>4654.8</v>
+      </c>
+      <c r="K6" s="31"/>
       <c r="L6" s="11" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="20">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="N6" s="15">
         <v>21</v>
@@ -3378,31 +4835,26 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="23">
-        <f>AVERAGE(M4:V4)</f>
+      <c r="C7" s="26">
         <v>2</v>
       </c>
-      <c r="D7" s="23">
-        <f>AVERAGE(M6:V6)</f>
-        <v>20.2</v>
-      </c>
-      <c r="E7" s="23">
-        <f>AVERAGE(M8:V8)</f>
-        <v>166.7</v>
-      </c>
-      <c r="F7" s="1">
-        <f>AVERAGE(M10:V10)</f>
-        <v>1306.8</v>
-      </c>
-      <c r="G7" s="1">
-        <f>AVERAGE(M12:V12)</f>
-        <v>10989.2</v>
-      </c>
-      <c r="K7" s="28">
+      <c r="D7" s="26">
+        <v>82.1</v>
+      </c>
+      <c r="E7" s="26">
+        <v>636.20000000000005</v>
+      </c>
+      <c r="F7" s="26">
+        <v>5198.7</v>
+      </c>
+      <c r="G7" s="26">
+        <v>37174.800000000003</v>
+      </c>
+      <c r="K7" s="31">
         <v>6</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -3440,7 +4892,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -3448,18 +4900,18 @@
         <v>1</v>
       </c>
       <c r="D8" s="23">
-        <v>1.77</v>
+        <v>2.69</v>
       </c>
       <c r="E8" s="23">
-        <v>2.11</v>
+        <v>2.71</v>
       </c>
       <c r="F8" s="1">
-        <v>2.2799999999999998</v>
+        <v>2.75</v>
       </c>
       <c r="G8" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="K8" s="28"/>
+        <v>2.74</v>
+      </c>
+      <c r="K8" s="31"/>
       <c r="L8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3495,7 +4947,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3516,7 +4968,7 @@
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="31">
         <v>8</v>
       </c>
       <c r="L9" s="11" t="s">
@@ -3554,7 +5006,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3573,7 +5025,7 @@
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="28"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="11" t="s">
         <v>7</v>
       </c>
@@ -3609,12 +5061,12 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="21">
-        <v>8.6325299999999991</v>
+        <v>14.77</v>
       </c>
       <c r="D11" s="21">
         <v>6.1762899999999998</v>
@@ -3628,7 +5080,7 @@
       <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="31">
         <v>10</v>
       </c>
       <c r="L11" s="11" t="s">
@@ -3666,33 +5118,28 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
-        <f>AVERAGE(B18:K18)</f>
+      <c r="C12" s="26">
         <v>3</v>
       </c>
-      <c r="D12" s="1">
-        <f>AVERAGE(B20:K20)</f>
-        <v>7.2</v>
-      </c>
-      <c r="E12" s="1">
-        <f>AVERAGE(B22:K22)</f>
-        <v>29.7</v>
-      </c>
-      <c r="F12" s="1">
-        <f>AVERAGE(B24:K24)</f>
-        <v>308.7</v>
-      </c>
-      <c r="G12" s="1">
-        <f>AVERAGE(B26:K26)</f>
-        <v>3543</v>
-      </c>
-      <c r="K12" s="29"/>
+      <c r="D12" s="26">
+        <v>10.7</v>
+      </c>
+      <c r="E12" s="26">
+        <v>33.5</v>
+      </c>
+      <c r="F12" s="26">
+        <v>163.5</v>
+      </c>
+      <c r="G12" s="26">
+        <v>1275.5</v>
+      </c>
+      <c r="K12" s="32"/>
       <c r="L12" s="12" t="s">
         <v>7</v>
       </c>
@@ -3728,50 +5175,45 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
-        <f>AVERAGE(B19:K19)</f>
+      <c r="C13" s="26">
         <v>17</v>
       </c>
-      <c r="D13" s="1">
-        <f>AVERAGE(B21:K21)</f>
-        <v>50.6</v>
-      </c>
-      <c r="E13" s="1">
-        <f>AVERAGE(B23:K23)</f>
-        <v>230.4</v>
-      </c>
-      <c r="F13" s="1">
-        <f>AVERAGE(B25:K25)</f>
-        <v>2457</v>
-      </c>
-      <c r="G13" s="1">
-        <f>AVERAGE(B27:K27)</f>
-        <v>28280</v>
+      <c r="D13" s="26">
+        <v>68</v>
+      </c>
+      <c r="E13" s="26">
+        <v>223.8</v>
+      </c>
+      <c r="F13" s="26">
+        <v>1120.5999999999999</v>
+      </c>
+      <c r="G13" s="26">
+        <v>8842.9</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="1">
         <v>3.65</v>
       </c>
-      <c r="D14" s="1">
-        <v>2.34</v>
+      <c r="D14" s="2">
+        <v>2.5499999999999998</v>
       </c>
       <c r="E14" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F14" s="1">
         <v>2.23</v>
       </c>
-      <c r="F14" s="1">
-        <v>2.4900000000000002</v>
-      </c>
       <c r="G14" s="1">
-        <v>2.66</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -3826,7 +5268,7 @@
       <c r="L17" s="24"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="28">
         <v>2</v>
       </c>
       <c r="B18" s="24">
@@ -3862,7 +5304,7 @@
       <c r="L18" s="24"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="24">
         <v>17</v>
       </c>
@@ -3896,7 +5338,7 @@
       <c r="L19" s="24"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="A20" s="28">
         <v>4</v>
       </c>
       <c r="B20" s="2">
@@ -3932,7 +5374,7 @@
       <c r="L20" s="24"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="2">
         <v>41</v>
       </c>
@@ -3966,7 +5408,7 @@
       <c r="L21" s="24"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="28">
         <v>6</v>
       </c>
       <c r="B22" s="2">
@@ -4002,7 +5444,7 @@
       <c r="L22" s="24"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="2">
         <v>217</v>
       </c>
@@ -4036,7 +5478,7 @@
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="28">
         <v>8</v>
       </c>
       <c r="B24" s="1">
@@ -4072,7 +5514,7 @@
       <c r="L24" s="24"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="2">
         <v>2373</v>
       </c>
@@ -4106,7 +5548,7 @@
       <c r="L25" s="24"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
+      <c r="A26" s="28">
         <v>10</v>
       </c>
       <c r="B26" s="2">
@@ -4142,7 +5584,7 @@
       <c r="L26" s="24"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="2">
         <v>41968</v>
       </c>
@@ -4179,10 +5621,68 @@
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>91</v>
+      </c>
       <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="26">
+        <v>2</v>
+      </c>
+      <c r="C31" s="26">
+        <v>2</v>
+      </c>
+      <c r="E31" s="26">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="F31" s="26">
+        <v>205.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="26">
+        <v>13.4</v>
+      </c>
+      <c r="C32" s="26">
+        <v>82.1</v>
+      </c>
+      <c r="E32" s="26">
+        <v>1628.2</v>
+      </c>
+      <c r="F32" s="26">
+        <v>9562.9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="26">
+        <v>79.8</v>
+      </c>
+      <c r="C33" s="26">
+        <v>636.20000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="26">
+        <v>626.29999999999995</v>
+      </c>
+      <c r="C34" s="26">
+        <v>5198.7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="26">
+        <v>4654.8</v>
+      </c>
+      <c r="C35" s="26">
+        <v>37174.800000000003</v>
+      </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
@@ -4656,11 +6156,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="K5:K6"/>
@@ -4668,14 +6170,13 @@
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A3:A5"/>
-    <mergeCell ref="K1:V1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>